<commit_message>
shop size is fixed
</commit_message>
<xml_diff>
--- a/OpenWorld/Resources/Armors.xlsx
+++ b/OpenWorld/Resources/Armors.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25050" windowHeight="8145" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25050" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="Armors" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="59">
   <si>
     <t>name</t>
   </si>
@@ -160,6 +160,48 @@
   </si>
   <si>
     <t>feet piece</t>
+  </si>
+  <si>
+    <t>Hood2</t>
+  </si>
+  <si>
+    <t>Mask2</t>
+  </si>
+  <si>
+    <t>Wizard Hat2</t>
+  </si>
+  <si>
+    <t>Steel Helmet2</t>
+  </si>
+  <si>
+    <t>Head bandages2</t>
+  </si>
+  <si>
+    <t>Blindfold of the damned2</t>
+  </si>
+  <si>
+    <t>Steel cauldrons2</t>
+  </si>
+  <si>
+    <t>Iron cauldrons2</t>
+  </si>
+  <si>
+    <t>Leather cauldrons2</t>
+  </si>
+  <si>
+    <t>Iron armor2</t>
+  </si>
+  <si>
+    <t>Leather armor2</t>
+  </si>
+  <si>
+    <t>Robes2</t>
+  </si>
+  <si>
+    <t>Steel armor2</t>
+  </si>
+  <si>
+    <t>Quilted coat2</t>
   </si>
 </sst>
 </file>
@@ -211,11 +253,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -433,7 +476,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -596,13 +641,13 @@
         <v>12</v>
       </c>
       <c r="D7" s="1">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F7" s="1">
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="G7" s="1">
         <v>5</v>
@@ -793,54 +838,334 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="2">
+        <v>3</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>3</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="1">
+        <v>3</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="1">
+        <v>-5</v>
+      </c>
+      <c r="E21" s="1">
+        <v>5</v>
+      </c>
+      <c r="F21" s="1">
+        <v>-5</v>
+      </c>
+      <c r="G21" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="1">
+        <v>5</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="1">
+        <v>5</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="1">
+        <v>7</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1">
+        <v>3</v>
+      </c>
+      <c r="G28" s="1">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="2">
+        <v>2</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C32" s="1"/>
     </row>
     <row r="33" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2369,7 +2694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixes regarding generation, now it works a bit differently
</commit_message>
<xml_diff>
--- a/OpenWorld/Resources/Armors.xlsx
+++ b/OpenWorld/Resources/Armors.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="47">
   <si>
     <t>name</t>
   </si>
@@ -162,46 +162,10 @@
     <t>feet piece</t>
   </si>
   <si>
-    <t>Hood2</t>
-  </si>
-  <si>
-    <t>Mask2</t>
-  </si>
-  <si>
-    <t>Wizard Hat2</t>
-  </si>
-  <si>
-    <t>Steel Helmet2</t>
-  </si>
-  <si>
-    <t>Head bandages2</t>
-  </si>
-  <si>
-    <t>Blindfold of the damned2</t>
-  </si>
-  <si>
-    <t>Steel cauldrons2</t>
-  </si>
-  <si>
-    <t>Iron cauldrons2</t>
-  </si>
-  <si>
-    <t>Leather cauldrons2</t>
-  </si>
-  <si>
-    <t>Iron armor2</t>
-  </si>
-  <si>
-    <t>Leather armor2</t>
-  </si>
-  <si>
-    <t>Robes2</t>
-  </si>
-  <si>
-    <t>Steel armor2</t>
-  </si>
-  <si>
-    <t>Quilted coat2</t>
+    <t>Gergő</t>
+  </si>
+  <si>
+    <t>Máté</t>
   </si>
 </sst>
 </file>
@@ -253,12 +217,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -477,7 +440,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -841,20 +804,20 @@
       <c r="A16" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>11</v>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D16" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" s="2">
         <v>0</v>
       </c>
       <c r="F16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" s="2">
         <v>0</v>
@@ -862,42 +825,42 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>14</v>
+        <v>45</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D17" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E17" s="2">
         <v>0</v>
       </c>
       <c r="F17" s="2">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G17" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>9</v>
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D18" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F18" s="2">
         <v>0</v>
@@ -907,215 +870,215 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>48</v>
+      <c r="A19" t="s">
+        <v>45</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="1">
-        <v>3</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-      <c r="F19" s="1">
+        <v>28</v>
+      </c>
+      <c r="D19" s="2">
         <v>2</v>
       </c>
-      <c r="G19" s="1">
-        <v>-1</v>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>49</v>
+      <c r="A20" t="s">
+        <v>45</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="1">
-        <v>1</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0</v>
-      </c>
-      <c r="F20" s="1">
-        <v>0</v>
-      </c>
-      <c r="G20" s="1">
+        <v>28</v>
+      </c>
+      <c r="D20" s="2">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>50</v>
+      <c r="A21" t="s">
+        <v>45</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="1">
-        <v>-5</v>
-      </c>
-      <c r="E21" s="1">
-        <v>5</v>
-      </c>
-      <c r="F21" s="1">
-        <v>-5</v>
-      </c>
-      <c r="G21" s="1">
-        <v>5</v>
+        <v>28</v>
+      </c>
+      <c r="D21" s="2">
+        <v>2</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>51</v>
+      <c r="A22" t="s">
+        <v>45</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="1">
-        <v>5</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0</v>
-      </c>
-      <c r="F22" s="1">
-        <v>1</v>
-      </c>
-      <c r="G22" s="1">
-        <v>-2</v>
+        <v>28</v>
+      </c>
+      <c r="D22" s="2">
+        <v>2</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>52</v>
+      <c r="A23" t="s">
+        <v>45</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" s="1">
-        <v>3</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0</v>
-      </c>
-      <c r="F23" s="1">
-        <v>1</v>
-      </c>
-      <c r="G23" s="1">
-        <v>-1</v>
+        <v>28</v>
+      </c>
+      <c r="D23" s="2">
+        <v>2</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>53</v>
+      <c r="A24" t="s">
+        <v>45</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="1">
-        <v>1</v>
-      </c>
-      <c r="E24" s="1">
-        <v>0</v>
-      </c>
-      <c r="F24" s="1">
-        <v>1</v>
-      </c>
-      <c r="G24" s="1">
+        <v>28</v>
+      </c>
+      <c r="D24" s="2">
+        <v>2</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0</v>
+      </c>
+      <c r="G24" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="2" t="s">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="1">
-        <v>5</v>
-      </c>
-      <c r="E25" s="1">
-        <v>0</v>
-      </c>
-      <c r="F25" s="1">
+      <c r="D25" s="2">
         <v>2</v>
       </c>
-      <c r="G25" s="1">
-        <v>-2</v>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>55</v>
+      <c r="A26" t="s">
+        <v>45</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="1">
-        <v>1</v>
-      </c>
-      <c r="E26" s="1">
-        <v>0</v>
-      </c>
-      <c r="F26" s="1">
-        <v>1</v>
-      </c>
-      <c r="G26" s="1">
-        <v>-1</v>
+      <c r="D26" s="2">
+        <v>2</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>56</v>
+      <c r="A27" t="s">
+        <v>45</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="1">
-        <v>1</v>
-      </c>
-      <c r="E27" s="1">
-        <v>0</v>
-      </c>
-      <c r="F27" s="1">
-        <v>0</v>
-      </c>
-      <c r="G27" s="1">
+      <c r="D27" s="2">
+        <v>2</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>57</v>
+      <c r="A28" t="s">
+        <v>45</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>17</v>
@@ -1123,22 +1086,22 @@
       <c r="C28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="1">
-        <v>7</v>
-      </c>
-      <c r="E28" s="1">
-        <v>0</v>
-      </c>
-      <c r="F28" s="1">
-        <v>3</v>
-      </c>
-      <c r="G28" s="1">
-        <v>-3</v>
+      <c r="D28" s="2">
+        <v>2</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>58</v>
+      <c r="A29" t="s">
+        <v>46</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>17</v>
@@ -1160,60 +1123,290 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="1"/>
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="2">
+        <v>2</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="1"/>
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="2">
+        <v>2</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" s="2">
+        <v>2</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="2">
+        <v>2</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="2">
+        <v>2</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" s="2">
+        <v>2</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="2">
+        <v>2</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" s="2">
+        <v>2</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" s="2">
+        <v>2</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0</v>
+      </c>
+      <c r="G38" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" s="2">
+        <v>2</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0</v>
+      </c>
+      <c r="G39" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="1"/>
       <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="1"/>
       <c r="C42" s="1"/>
-    </row>
-    <row r="43" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="1"/>
       <c r="C43" s="1"/>
-    </row>
-    <row r="44" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="1"/>
       <c r="C44" s="1"/>
-    </row>
-    <row r="45" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="1"/>
       <c r="C45" s="1"/>
-    </row>
-    <row r="46" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C48" s="1"/>
     </row>
     <row r="49" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
new items added, acolyte renamed to outcast
</commit_message>
<xml_diff>
--- a/OpenWorld/Resources/Armors.xlsx
+++ b/OpenWorld/Resources/Armors.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Suli\GitHub\CppProjects\DnD\OpenWorld\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epolako\repos\DnD\OpenWorld\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66CD06F-BC54-4029-8F6D-8AA3AE6BD952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25050" windowHeight="8145"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Armors" sheetId="2" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="74">
   <si>
     <t>name</t>
   </si>
@@ -60,54 +61,27 @@
     <t>Hood</t>
   </si>
   <si>
-    <t>Mage,Acolyte,Ranger,Rouge,Slayer</t>
-  </si>
-  <si>
     <t>head piece</t>
   </si>
   <si>
     <t>Mask</t>
   </si>
   <si>
-    <t>Acolyte,Ranger,Rouge,Slayer</t>
-  </si>
-  <si>
     <t>Wizard Hat</t>
   </si>
   <si>
     <t>Steel Helmet</t>
   </si>
   <si>
-    <t>Warrior,Acolyte</t>
-  </si>
-  <si>
     <t>Head bandages</t>
   </si>
   <si>
-    <t>Warrior,Ranger,Rouge,Acolyte,Mage,Slayer</t>
-  </si>
-  <si>
     <t>Blindfold of the damned</t>
   </si>
   <si>
-    <t>Acolyte,Slayer</t>
-  </si>
-  <si>
-    <t>Steel cauldrons</t>
-  </si>
-  <si>
     <t>shoulder piece</t>
   </si>
   <si>
-    <t>Iron cauldrons</t>
-  </si>
-  <si>
-    <t>Leather cauldrons</t>
-  </si>
-  <si>
-    <t>Warrior,Ranger,Rouge,Acolyte</t>
-  </si>
-  <si>
     <t>Iron armor</t>
   </si>
   <si>
@@ -123,9 +97,6 @@
     <t>Steel armor</t>
   </si>
   <si>
-    <t>Quilted coat</t>
-  </si>
-  <si>
     <t>healing</t>
   </si>
   <si>
@@ -162,17 +133,128 @@
     <t>feet piece</t>
   </si>
   <si>
-    <t>Gergő</t>
-  </si>
-  <si>
-    <t>Máté</t>
+    <t>Steel pauldrons</t>
+  </si>
+  <si>
+    <t>Iron pauldrons</t>
+  </si>
+  <si>
+    <t>Leather pauldrons</t>
+  </si>
+  <si>
+    <t>Padded Gambeson</t>
+  </si>
+  <si>
+    <t>Leather Scale coat</t>
+  </si>
+  <si>
+    <t>Chainmail</t>
+  </si>
+  <si>
+    <t>Great Helm</t>
+  </si>
+  <si>
+    <t>Chain Hood</t>
+  </si>
+  <si>
+    <t>Armet Helm</t>
+  </si>
+  <si>
+    <t>Leather Gloves</t>
+  </si>
+  <si>
+    <t>Iron Brace</t>
+  </si>
+  <si>
+    <t>Iron Gauntlet</t>
+  </si>
+  <si>
+    <t>Darksteel Claws</t>
+  </si>
+  <si>
+    <t>Leather Boots</t>
+  </si>
+  <si>
+    <t>Sandal</t>
+  </si>
+  <si>
+    <t>Heavy Boots</t>
+  </si>
+  <si>
+    <t>Steel Leg Armor</t>
+  </si>
+  <si>
+    <t>Cloak</t>
+  </si>
+  <si>
+    <t>Hide Armor</t>
+  </si>
+  <si>
+    <t>Fur Armor</t>
+  </si>
+  <si>
+    <t>Ring of Power</t>
+  </si>
+  <si>
+    <t>Boots of Swiftness</t>
+  </si>
+  <si>
+    <t>Ranger</t>
+  </si>
+  <si>
+    <t>Slayer</t>
+  </si>
+  <si>
+    <t>Rouge</t>
+  </si>
+  <si>
+    <t>Warrior</t>
+  </si>
+  <si>
+    <t>Belt of Chad</t>
+  </si>
+  <si>
+    <t>Mage,Outcast,Ranger,Rouge,Slayer</t>
+  </si>
+  <si>
+    <t>Outcast,Ranger,Rouge,Slayer</t>
+  </si>
+  <si>
+    <t>Warrior,Outcast</t>
+  </si>
+  <si>
+    <t>Warrior,Ranger,Rouge,Outcast,Mage,Slayer</t>
+  </si>
+  <si>
+    <t>Warrior,Ranger,Rouge,Outcast</t>
+  </si>
+  <si>
+    <t>Warrior,Outcast,Rouge,Ranger</t>
+  </si>
+  <si>
+    <t>Outcast</t>
+  </si>
+  <si>
+    <t>Hood of the crowd</t>
+  </si>
+  <si>
+    <t>Glorious Chestplate</t>
+  </si>
+  <si>
+    <t>Jester Robes</t>
+  </si>
+  <si>
+    <t>Scawl of the night</t>
+  </si>
+  <si>
+    <t>Burned Cape</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +278,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -217,14 +306,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normál" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -436,11 +526,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:G29"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -456,25 +546,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -483,10 +573,10 @@
         <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -503,13 +593,13 @@
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2">
         <v>3</v>
@@ -526,13 +616,13 @@
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -549,13 +639,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1">
         <v>3</v>
@@ -572,13 +662,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -595,13 +685,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -618,13 +708,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="D8" s="1">
         <v>5</v>
@@ -641,13 +731,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="D9" s="1">
         <v>3</v>
@@ -664,13 +754,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -687,13 +777,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D11" s="1">
         <v>5</v>
@@ -710,13 +800,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
@@ -733,13 +823,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -756,13 +846,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D14" s="1">
         <v>7</v>
@@ -779,13 +869,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D15" s="2">
         <v>2</v>
@@ -802,13 +892,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D16" s="2">
         <v>2</v>
@@ -825,13 +915,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D17" s="2">
         <v>2</v>
@@ -848,13 +938,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D18" s="2">
         <v>2</v>
@@ -871,13 +961,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D19" s="2">
         <v>2</v>
@@ -894,13 +984,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D20" s="2">
         <v>2</v>
@@ -917,13 +1007,13 @@
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D21" s="2">
         <v>2</v>
@@ -943,10 +1033,10 @@
         <v>45</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D22" s="2">
         <v>2</v>
@@ -963,13 +1053,13 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D23" s="2">
         <v>2</v>
@@ -986,13 +1076,13 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D24" s="2">
         <v>2</v>
@@ -1009,13 +1099,13 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D25" s="2">
         <v>2</v>
@@ -1032,13 +1122,13 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D26" s="2">
         <v>2</v>
@@ -1055,13 +1145,13 @@
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D27" s="2">
         <v>2</v>
@@ -1078,13 +1168,13 @@
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D28" s="2">
         <v>2</v>
@@ -1101,13 +1191,13 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D29" s="2">
         <v>2</v>
@@ -1124,13 +1214,13 @@
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D30" s="2">
         <v>2</v>
@@ -1147,13 +1237,13 @@
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D31" s="2">
         <v>2</v>
@@ -1170,19 +1260,19 @@
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D32" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E32" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F32" s="2">
         <v>0</v>
@@ -1193,13 +1283,13 @@
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D33" s="2">
         <v>2</v>
@@ -1216,13 +1306,13 @@
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D34" s="2">
         <v>2</v>
@@ -1239,13 +1329,13 @@
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D35" s="2">
         <v>2</v>
@@ -1262,13 +1352,13 @@
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D36" s="2">
         <v>2</v>
@@ -1285,13 +1375,13 @@
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D37" s="2">
         <v>2</v>
@@ -1308,13 +1398,13 @@
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D38" s="2">
         <v>2</v>
@@ -1331,13 +1421,13 @@
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D39" s="2">
         <v>2</v>
@@ -2867,11 +2957,11 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Types!$B$2:$B$7</xm:f>
           </x14:formula1>
@@ -2884,7 +2974,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2901,13 +2991,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2915,10 +3005,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2926,23 +3016,23 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -2950,23 +3040,23 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>